<commit_message>
nvm final commit 8/11
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F7DFC75-7D5E-4E05-98C5-48F40494DDED}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30757B94-77A1-4D4A-ADD7-1D1489F483DE}"/>
   <bookViews>
     <workbookView xWindow="-6105" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -400,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,13 +462,52 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -477,63 +516,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,10 +530,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFDDBC7"/>
       <color rgb="FFD1E5F0"/>
       <color rgb="FF4393C3"/>
       <color rgb="FFD6604D"/>
-      <color rgb="FFFDDBC7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -558,6 +545,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,15 +817,15 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" customWidth="1"/>
     <col min="2" max="2" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="45" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="45"/>
+    <col min="3" max="3" width="11.90625" style="33" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="33"/>
     <col min="8" max="8" width="3.81640625" customWidth="1"/>
     <col min="9" max="9" width="19.08984375" customWidth="1"/>
   </cols>
@@ -849,13 +840,13 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="26" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="4"/>
@@ -870,15 +861,19 @@
       <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="43"/>
+      <c r="D2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="31"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -887,31 +882,31 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="35"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="36"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="K4" s="26"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="34" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -920,45 +915,43 @@
       <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="35"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="24"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="35"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="24"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="34" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="4"/>
@@ -966,22 +959,22 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="23"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="34" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -993,14 +986,14 @@
       <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1010,14 +1003,14 @@
       <c r="D10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="35"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="21"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -1027,35 +1020,35 @@
       <c r="D11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="4"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="23"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="25"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="34" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1067,10 +1060,10 @@
       <c r="D13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="44" t="s">
+      <c r="E13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="32" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="9"/>
@@ -1080,7 +1073,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="9" t="s">
         <v>27</v>
       </c>
@@ -1090,10 +1083,10 @@
       <c r="D14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="41" t="s">
+      <c r="E14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="29" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="9"/>
@@ -1103,16 +1096,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="35" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="24" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="9"/>
@@ -1122,16 +1115,16 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="23"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="42" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="30" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="9"/>
@@ -1141,7 +1134,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="34" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1150,60 +1143,60 @@
       <c r="C17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="35"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="35"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="35"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="23"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="34" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1215,27 +1208,27 @@
       <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="35"/>
+      <c r="E21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="24"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="23"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="25" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="4"/>

</xml_diff>

<commit_message>
Results for Nest Site High / Low where all AMBIGUOUS nesting species (those that nest both HIGH and LOW) were removed.
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F10452-DC64-46DF-B936-FA5F89DC0A17}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4EA1D75-7B82-499A-BC08-C3A33C3E2935}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -451,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,9 +531,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,43 +540,43 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -877,15 +874,15 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" customWidth="1"/>
     <col min="2" max="2" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="28" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="28"/>
+    <col min="3" max="3" width="11.90625" style="27" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="27"/>
     <col min="8" max="8" width="3.81640625" customWidth="1"/>
     <col min="9" max="9" width="17.7265625" customWidth="1"/>
   </cols>
@@ -921,10 +918,10 @@
       <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="26"/>
@@ -933,7 +930,7 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -950,7 +947,7 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="32"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
@@ -966,7 +963,7 @@
       <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -985,7 +982,7 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +999,7 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="33"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
@@ -1019,7 +1016,7 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="32"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1031,7 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1053,7 +1050,7 @@
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
@@ -1070,7 +1067,7 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="33"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
@@ -1083,11 +1080,11 @@
       <c r="E11" s="8"/>
       <c r="F11" s="19"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="32"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
@@ -1101,14 +1098,14 @@
       <c r="F12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="37" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="38"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1123,17 +1120,15 @@
       <c r="E13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="35" t="s">
+      <c r="F13" s="42"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="30" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
@@ -1149,14 +1144,14 @@
       <c r="F14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="35" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
@@ -1168,14 +1163,14 @@
       <c r="F15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="35" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="32"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="6" t="s">
         <v>27</v>
       </c>
@@ -1187,14 +1182,14 @@
       <c r="F16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="35" t="s">
+      <c r="G16" s="4"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1207,13 +1202,13 @@
       <c r="E17" s="8"/>
       <c r="F17" s="19"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="36" t="s">
+      <c r="H17" s="36"/>
+      <c r="I17" s="31" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="9" t="s">
         <v>30</v>
       </c>
@@ -1228,7 +1223,7 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="9" t="s">
         <v>31</v>
       </c>
@@ -1243,7 +1238,7 @@
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="32"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
@@ -1258,7 +1253,7 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1279,7 +1274,7 @@
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="32"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="6" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
small edits to lambda script
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4EA1D75-7B82-499A-BC08-C3A33C3E2935}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BC3B12B-5CBF-4751-BCC0-5A2F8B90843B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -387,32 +387,286 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
@@ -420,12 +674,96 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
@@ -435,13 +773,114 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -451,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,9 +901,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -474,36 +910,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -513,15 +925,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -530,9 +936,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -546,19 +949,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,13 +973,152 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -602,10 +1144,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -874,20 +1412,22 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="27" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="27"/>
-    <col min="8" max="8" width="3.81640625" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" style="39" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="39"/>
+    <col min="7" max="7" width="8.7265625" style="31"/>
+    <col min="8" max="8" width="3.81640625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,403 +1437,403 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="38"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="K4" s="16"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="72"/>
+      <c r="E6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="18" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="38"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="39"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="38"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="40" t="s">
+      <c r="G12" s="30"/>
+      <c r="H12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="41"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="30" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="30" t="s">
+      <c r="G14" s="30"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="19" t="s">
+      <c r="D15" s="66"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="30" t="s">
+      <c r="G15" s="30"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="38"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="25" t="s">
+      <c r="D16" s="61"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="30" t="s">
+      <c r="G16" s="30"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="31" t="s">
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="39"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="39"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="38"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="38"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
+      <c r="D22" s="63"/>
+      <c r="E22" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I24" t="s">
+      <c r="I24" s="31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1308,5 +1848,6 @@
     <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-assessed all results according to significant == alpha < 0.05, and notable == alpha < 0.15 & 85% CI does NOT overlap 0. updated results table
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BC3B12B-5CBF-4751-BCC0-5A2F8B90843B}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95CF803B-12B1-4A47-BED0-9B8AEE1C51CE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Longevity</t>
   </si>
   <si>
-    <t>Developmental Mode (altruistic)</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -171,6 +168,15 @@
   </si>
   <si>
     <t>Significantly positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">significant - CI shouldn't overlap 0 at 95. if CI doesn't overlap 0 at 85… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">these are arbitrary thresholds no matter what… --&gt; use 85 CI as an arbitrary checkpoint (for ourselves) --&gt; are they too overlapping? Or can we say that it's a trend, but not a notable one. </t>
+  </si>
+  <si>
+    <t>Developmental Mode (Altricial = 0)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,8 +236,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -886,11 +898,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -940,9 +965,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -964,6 +986,150 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -979,146 +1145,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1129,8 +1162,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD1E5F0"/>
       <color rgb="FFFDDBC7"/>
-      <color rgb="FFD1E5F0"/>
       <color rgb="FF4393C3"/>
       <color rgb="FFD6604D"/>
     </mruColors>
@@ -1144,6 +1177,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1409,22 +1446,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="33.90625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="39" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="39"/>
-    <col min="7" max="7" width="8.7265625" style="31"/>
-    <col min="8" max="8" width="3.81640625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="31"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="32" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="32"/>
+    <col min="8" max="8" width="3.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1437,18 +1473,18 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4"/>
@@ -1461,380 +1497,383 @@
       <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="E2" s="78"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="72" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="26"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="73"/>
+      <c r="B4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="K4" s="33"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="36" t="s">
+      <c r="D6" s="65"/>
+      <c r="E6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="47"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="26"/>
-      <c r="B8" s="40" t="s">
+      <c r="A8" s="73"/>
+      <c r="B8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="61"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="72" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="74"/>
+      <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="42" t="s">
+      <c r="A11" s="74"/>
+      <c r="B11" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="79"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="73"/>
+      <c r="B12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="26"/>
-      <c r="B12" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="28" t="s">
+      <c r="G12" s="24"/>
+      <c r="H12" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="29"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
+      <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="74"/>
+      <c r="B14" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="29" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="18" t="s">
-        <v>43</v>
+      <c r="G14" s="24"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="74"/>
+      <c r="B15" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="59"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="18" t="s">
-        <v>42</v>
+      <c r="G15" s="24"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="26"/>
-      <c r="B16" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="43" t="s">
+      <c r="A16" s="73"/>
+      <c r="B16" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="6"/>
       <c r="F16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="25" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="C17" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="74"/>
+      <c r="B18" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C18" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="55" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="74"/>
+      <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="7" t="s">
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="73"/>
+      <c r="B20" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C20" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="26"/>
-      <c r="B20" s="40" t="s">
+      <c r="D20" s="54"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="B21" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="41" t="s">
+      <c r="D21" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="77"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="71"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="73"/>
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="65"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="26"/>
-      <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63" t="s">
+      <c r="D22" s="56"/>
+      <c r="E22" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I24" s="31" t="s">
-        <v>38</v>
+    </row>
+    <row r="27" spans="1:10" ht="174" x14ac:dyDescent="0.35">
+      <c r="I27" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="71" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redid figures and made bar plots for UN!
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95CF803B-12B1-4A47-BED0-9B8AEE1C51CE}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E49D5F6C-1BA7-4CDE-8170-A0338FE00BB1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">these are arbitrary thresholds no matter what… --&gt; use 85 CI as an arbitrary checkpoint (for ourselves) --&gt; are they too overlapping? Or can we say that it's a trend, but not a notable one. </t>
   </si>
   <si>
-    <t>Developmental Mode (Altricial = 0)</t>
+    <t>Developmental Mode (Altricial = 1)</t>
   </si>
 </sst>
 </file>
@@ -915,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1130,6 +1130,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,15 +1150,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1449,7 +1446,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1497,14 +1494,14 @@
       <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="78"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="15"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1521,7 +1518,7 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="73"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="33" t="s">
         <v>10</v>
       </c>
@@ -1537,7 +1534,7 @@
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="74" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -1556,7 +1553,7 @@
       <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="74"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1573,7 +1570,7 @@
       <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="35" t="s">
         <v>16</v>
       </c>
@@ -1590,7 +1587,7 @@
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="73"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="33" t="s">
         <v>17</v>
       </c>
@@ -1605,7 +1602,7 @@
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1624,7 +1621,7 @@
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="74"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="35" t="s">
         <v>20</v>
       </c>
@@ -1641,14 +1638,14 @@
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="74"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="79"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="42"/>
       <c r="F11" s="61"/>
       <c r="G11" s="24"/>
@@ -1656,7 +1653,7 @@
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="73"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="33" t="s">
         <v>46</v>
       </c>
@@ -1671,13 +1668,13 @@
         <v>11</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="75" t="s">
+      <c r="H12" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="76"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="74" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1700,7 +1697,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="74"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="35" t="s">
         <v>25</v>
       </c>
@@ -1723,7 +1720,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="74"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="35" t="s">
         <v>35</v>
       </c>
@@ -1742,7 +1739,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="73"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="33" t="s">
         <v>26</v>
       </c>
@@ -1761,7 +1758,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="74" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="34" t="s">
@@ -1780,7 +1777,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="74"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="48" t="s">
         <v>29</v>
       </c>
@@ -1795,7 +1792,7 @@
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="74"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1810,7 +1807,7 @@
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
+      <c r="A20" s="75"/>
       <c r="B20" s="33" t="s">
         <v>31</v>
       </c>
@@ -1825,7 +1822,7 @@
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="74" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="34" t="s">
@@ -1837,7 +1834,7 @@
       <c r="D21" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="77"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="58"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
@@ -1845,7 +1842,7 @@
       <c r="J21" s="71"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="73"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="5" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
new script for phyloglm & UN models
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E49D5F6C-1BA7-4CDE-8170-A0338FE00BB1}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C178B9C-4E0B-4BD5-AFDF-D75555BACC3E}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="300" windowWidth="9110" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -176,7 +177,7 @@
     <t xml:space="preserve">these are arbitrary thresholds no matter what… --&gt; use 85 CI as an arbitrary checkpoint (for ourselves) --&gt; are they too overlapping? Or can we say that it's a trend, but not a notable one. </t>
   </si>
   <si>
-    <t>Developmental Mode (Altricial = 1)</t>
+    <t xml:space="preserve">Life </t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Density Plots --> redone.
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C178B9C-4E0B-4BD5-AFDF-D75555BACC3E}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8D06E7-1F2A-4D94-91F5-4F25317F4271}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="300" windowWidth="9110" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="after phyloglm" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Dim Light Vision</t>
   </si>
   <si>
-    <t>Dominant Vocal Frequency</t>
-  </si>
-  <si>
     <t>(+)</t>
   </si>
   <si>
@@ -177,14 +174,29 @@
     <t xml:space="preserve">these are arbitrary thresholds no matter what… --&gt; use 85 CI as an arbitrary checkpoint (for ourselves) --&gt; are they too overlapping? Or can we say that it's a trend, but not a notable one. </t>
   </si>
   <si>
-    <t xml:space="preserve">Life </t>
+    <t>Peak Vocal Frequency</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developmental Mode  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN goes back to being non-significant --&gt; ok cool! Consistent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developmental Mode </t>
+  </si>
+  <si>
+    <t>becomes (-)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +217,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +260,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="53">
     <border>
@@ -916,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1151,6 +1174,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,10 +1192,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD6604D"/>
       <color rgb="FFD1E5F0"/>
       <color rgb="FFFDDBC7"/>
       <color rgb="FF4393C3"/>
-      <color rgb="FFD6604D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1446,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1521,10 +1553,10 @@
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="75"/>
       <c r="B4" s="33" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="37"/>
@@ -1536,13 +1568,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="27" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="31" t="s">
@@ -1556,14 +1588,14 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="76"/>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="65"/>
       <c r="E6" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="24"/>
@@ -1573,10 +1605,10 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="76"/>
       <c r="B7" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="40"/>
@@ -1590,10 +1622,10 @@
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="75"/>
       <c r="B8" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="54"/>
@@ -1604,10 +1636,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C9" s="46" t="s">
         <v>7</v>
@@ -1624,13 +1656,13 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="76"/>
       <c r="B10" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="62"/>
@@ -1641,10 +1673,10 @@
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="76"/>
       <c r="B11" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="42"/>
@@ -1656,30 +1688,30 @@
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="75"/>
       <c r="B12" s="33" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>7</v>
@@ -1694,76 +1726,76 @@
       <c r="G13" s="24"/>
       <c r="H13" s="19"/>
       <c r="I13" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="76"/>
       <c r="B14" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="20"/>
       <c r="I14" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="76"/>
       <c r="B15" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="59"/>
       <c r="E15" s="40"/>
       <c r="F15" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="21"/>
       <c r="I15" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="75"/>
       <c r="B16" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="6"/>
       <c r="F16" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="22"/>
       <c r="I16" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="46" t="s">
         <v>7</v>
@@ -1774,13 +1806,13 @@
       <c r="G17" s="24"/>
       <c r="H17" s="23"/>
       <c r="I17" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="76"/>
       <c r="B18" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="55" t="s">
         <v>7</v>
@@ -1795,7 +1827,7 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="76"/>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>7</v>
@@ -1810,7 +1842,7 @@
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="75"/>
       <c r="B20" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="44" t="s">
         <v>7</v>
@@ -1824,10 +1856,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>32</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>33</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>7</v>
@@ -1845,17 +1877,17 @@
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="75"/>
       <c r="B22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="56"/>
       <c r="E22" s="56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
@@ -1863,15 +1895,477 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="I27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="71" t="s">
         <v>44</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4268394-C4E6-4A65-A495-8A18F9709312}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="32" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="32"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="3.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="67"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="75"/>
+      <c r="B4" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+      <c r="A6" s="76"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="65"/>
+      <c r="E6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
+      <c r="B7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="75"/>
+      <c r="B8" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="76"/>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="76"/>
+      <c r="B11" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="75"/>
+      <c r="B12" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="56"/>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="78"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="76"/>
+      <c r="B14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="76"/>
+      <c r="B15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="59"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="75"/>
+      <c r="B16" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="54"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="76"/>
+      <c r="B18" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="76"/>
+      <c r="B19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="75"/>
+      <c r="B20" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="54"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="72"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="71"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="75"/>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="174" x14ac:dyDescent="0.35">
+      <c r="I27" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="J27" s="71" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking ranges for UAI and MUTI
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8D06E7-1F2A-4D94-91F5-4F25317F4271}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96091677-5175-44B1-BF04-8FD48FB79255}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="48">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -177,19 +177,10 @@
     <t>Peak Vocal Frequency</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Developmental Mode  </t>
   </si>
   <si>
-    <t xml:space="preserve">UN goes back to being non-significant --&gt; ok cool! Consistent </t>
-  </si>
-  <si>
     <t xml:space="preserve">Developmental Mode </t>
-  </si>
-  <si>
-    <t>becomes (-)</t>
   </si>
 </sst>
 </file>
@@ -223,7 +214,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,12 +251,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="53">
     <border>
@@ -939,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1175,13 +1160,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,9 +1189,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFDDBC7"/>
       <color rgb="FFD6604D"/>
       <color rgb="FFD1E5F0"/>
-      <color rgb="FFFDDBC7"/>
       <color rgb="FF4393C3"/>
     </mruColors>
   </colors>
@@ -1688,7 +1685,7 @@
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="75"/>
       <c r="B12" s="33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>7</v>
@@ -1926,7 +1923,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,9 +2005,7 @@
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="37"/>
-      <c r="F4" s="79" t="s">
-        <v>46</v>
-      </c>
+      <c r="F4" s="81"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -2035,7 +2030,7 @@
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:11" ht="101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="76"/>
       <c r="B6" s="7" t="s">
         <v>14</v>
@@ -2047,12 +2042,8 @@
       <c r="E6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>48</v>
-      </c>
+      <c r="F6" s="79"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
     </row>
@@ -2066,10 +2057,10 @@
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="40"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="31" t="s">
-        <v>50</v>
-      </c>
+      <c r="F7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="80"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
     </row>
@@ -2088,7 +2079,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="74" t="s">
         <v>17</v>
       </c>
@@ -2102,14 +2093,12 @@
         <v>7</v>
       </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="79" t="s">
-        <v>46</v>
-      </c>
+      <c r="F9" s="82"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="76"/>
       <c r="B10" s="35" t="s">
         <v>19</v>
@@ -2121,9 +2110,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="42"/>
-      <c r="F10" s="79" t="s">
-        <v>46</v>
-      </c>
+      <c r="F10" s="83"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
@@ -2136,9 +2123,9 @@
       <c r="C11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="42"/>
-      <c r="F11" s="61"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -2146,7 +2133,7 @@
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="75"/>
       <c r="B12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>7</v>
@@ -2155,7 +2142,7 @@
       <c r="E12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="24"/>
@@ -2239,8 +2226,8 @@
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="79" t="s">
-        <v>46</v>
+      <c r="F16" s="84" t="s">
+        <v>10</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="22"/>
@@ -2282,7 +2269,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="76"/>
       <c r="B19" s="7" t="s">
         <v>29</v>
@@ -2292,9 +2279,7 @@
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
-      <c r="F19" s="79" t="s">
-        <v>46</v>
-      </c>
+      <c r="F19" s="85"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
@@ -2309,9 +2294,7 @@
       </c>
       <c r="D20" s="54"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="79" t="s">
-        <v>46</v>
-      </c>
+      <c r="F20" s="81"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>

</xml_diff>

<commit_message>
checked some 85% CI
</commit_message>
<xml_diff>
--- a/Results/Results Simplified.xlsx
+++ b/Results/Results Simplified.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96091677-5175-44B1-BF04-8FD48FB79255}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{331E838A-C464-4237-BA59-34EC520F3C09}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="after phyloglm" sheetId="2" r:id="rId2"/>
+    <sheet name="including &quot;only&quot; high and low" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="51">
   <si>
     <t>Trait Grouping</t>
   </si>
@@ -181,6 +182,15 @@
   </si>
   <si>
     <t xml:space="preserve">Developmental Mode </t>
+  </si>
+  <si>
+    <t>UAI ONLY</t>
+  </si>
+  <si>
+    <t>MUTI ONLY</t>
+  </si>
+  <si>
+    <t>UN ONLY</t>
   </si>
 </sst>
 </file>
@@ -924,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1145,6 +1155,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,25 +1176,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1189,10 +1205,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD6604D"/>
+      <color rgb="FF4393C3"/>
       <color rgb="FFFDDBC7"/>
-      <color rgb="FFD6604D"/>
       <color rgb="FFD1E5F0"/>
-      <color rgb="FF4393C3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1531,7 +1547,7 @@
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1548,7 +1564,7 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="75"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="33" t="s">
         <v>45</v>
       </c>
@@ -1564,7 +1580,7 @@
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="76" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -1583,7 +1599,7 @@
       <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="76"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1616,7 @@
       <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="76"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="35" t="s">
         <v>15</v>
       </c>
@@ -1617,7 +1633,7 @@
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="75"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="33" t="s">
         <v>16</v>
       </c>
@@ -1632,7 +1648,7 @@
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="76" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1651,7 +1667,7 @@
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="76"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="35" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1684,7 @@
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="76"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="35" t="s">
         <v>20</v>
       </c>
@@ -1683,7 +1699,7 @@
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="75"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="33" t="s">
         <v>47</v>
       </c>
@@ -1698,13 +1714,13 @@
         <v>10</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="78"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="76" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1727,7 +1743,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="76"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="35" t="s">
         <v>24</v>
       </c>
@@ -1750,7 +1766,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="76"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="35" t="s">
         <v>34</v>
       </c>
@@ -1769,7 +1785,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="75"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="33" t="s">
         <v>25</v>
       </c>
@@ -1788,7 +1804,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="34" t="s">
@@ -1807,7 +1823,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="76"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="48" t="s">
         <v>28</v>
       </c>
@@ -1822,7 +1838,7 @@
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="76"/>
+      <c r="A19" s="78"/>
       <c r="B19" s="7" t="s">
         <v>29</v>
       </c>
@@ -1837,7 +1853,7 @@
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="75"/>
+      <c r="A20" s="77"/>
       <c r="B20" s="33" t="s">
         <v>30</v>
       </c>
@@ -1852,7 +1868,7 @@
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="76" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="34" t="s">
@@ -1872,7 +1888,7 @@
       <c r="J21" s="71"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="75"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1922,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4268394-C4E6-4A65-A495-8A18F9709312}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1979,7 +1995,7 @@
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1996,7 +2012,7 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="75"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="33" t="s">
         <v>45</v>
       </c>
@@ -2005,14 +2021,14 @@
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="37"/>
-      <c r="F4" s="81"/>
+      <c r="F4" s="50"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="76" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -2031,7 +2047,7 @@
       <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="76"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2042,13 +2058,13 @@
       <c r="E6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="74"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="76"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="35" t="s">
         <v>15</v>
       </c>
@@ -2060,12 +2076,12 @@
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="80"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="75"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="33" t="s">
         <v>16</v>
       </c>
@@ -2080,7 +2096,7 @@
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="76" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -2093,13 +2109,13 @@
         <v>7</v>
       </c>
       <c r="E9" s="25"/>
-      <c r="F9" s="82"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="76"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="35" t="s">
         <v>19</v>
       </c>
@@ -2110,13 +2126,13 @@
         <v>10</v>
       </c>
       <c r="E10" s="42"/>
-      <c r="F10" s="83"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="76"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="35" t="s">
         <v>20</v>
       </c>
@@ -2131,7 +2147,7 @@
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="75"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="33" t="s">
         <v>46</v>
       </c>
@@ -2146,13 +2162,13 @@
         <v>10</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="78"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="76" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -2175,7 +2191,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="76"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="35" t="s">
         <v>24</v>
       </c>
@@ -2198,7 +2214,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="76"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="35" t="s">
         <v>34</v>
       </c>
@@ -2217,7 +2233,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="75"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="33" t="s">
         <v>25</v>
       </c>
@@ -2226,7 +2242,7 @@
       </c>
       <c r="D16" s="54"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="84" t="s">
+      <c r="F16" s="75" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="24"/>
@@ -2236,7 +2252,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="34" t="s">
@@ -2255,7 +2271,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="76"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="48" t="s">
         <v>28</v>
       </c>
@@ -2270,7 +2286,7 @@
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="76"/>
+      <c r="A19" s="78"/>
       <c r="B19" s="7" t="s">
         <v>29</v>
       </c>
@@ -2279,13 +2295,13 @@
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
-      <c r="F19" s="85"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="75"/>
+      <c r="A20" s="77"/>
       <c r="B20" s="33" t="s">
         <v>30</v>
       </c>
@@ -2294,13 +2310,13 @@
       </c>
       <c r="D20" s="54"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="81"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="76" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="34" t="s">
@@ -2320,7 +2336,7 @@
       <c r="J21" s="71"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="75"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
@@ -2364,4 +2380,484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322374B7-AB63-4811-83EF-F66B22DE617F}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="32" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="32"/>
+    <col min="7" max="7" width="9.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="67"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="77"/>
+      <c r="B4" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="78"/>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="65"/>
+      <c r="E6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="74"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="78"/>
+      <c r="B7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="77"/>
+      <c r="B8" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="78"/>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="78"/>
+      <c r="B11" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="59"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="77"/>
+      <c r="B12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="56"/>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="68" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="82"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="78"/>
+      <c r="B14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="82"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="78"/>
+      <c r="B15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="59"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="77"/>
+      <c r="B16" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="54"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="82"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="82"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="78"/>
+      <c r="B18" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="78"/>
+      <c r="B19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="77"/>
+      <c r="B20" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="54"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="72"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="71"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="77"/>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="80"/>
+    </row>
+    <row r="27" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="B27" s="19"/>
+      <c r="C27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="71"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="20"/>
+      <c r="C28" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="21"/>
+      <c r="C29" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="B30" s="22"/>
+      <c r="C30" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="23"/>
+      <c r="C31" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>